<commit_message>
TÉNYLEG fixed routing error
</commit_message>
<xml_diff>
--- a/Other/HACKEDmap.xlsx
+++ b/Other/HACKEDmap.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62DB3EE3-8E39-4986-B56B-8D248943BA15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8181A18B-4D03-4EC1-A4A1-D83B2FECAE32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -548,67 +548,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="193">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1162,6 +1106,61 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1412,69 +1411,69 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E10DE2FA-2DD2-4EBF-BD63-DCCFA5FF4AD0}" name="Új_szöveges_dokumentum__2" displayName="Új_szöveges_dokumentum__2" ref="B2:BI63" tableType="queryTable" totalsRowShown="0" headerRowDxfId="190" dataDxfId="189">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E10DE2FA-2DD2-4EBF-BD63-DCCFA5FF4AD0}" name="Új_szöveges_dokumentum__2" displayName="Új_szöveges_dokumentum__2" ref="B2:BI63" tableType="queryTable" totalsRowShown="0" headerRowDxfId="183" dataDxfId="182">
   <autoFilter ref="B2:BI63" xr:uid="{DE6A2C29-F277-44C9-8C93-967D97F43468}"/>
   <tableColumns count="60">
-    <tableColumn id="1" xr3:uid="{571AD5BC-C083-42BF-B574-6B0FBB157DF0}" uniqueName="1" name="Oszlop1" queryTableFieldId="1" dataDxfId="188"/>
-    <tableColumn id="2" xr3:uid="{C9DF9092-1CA9-40C8-A22F-7A8869D9424A}" uniqueName="2" name="Oszlop2" queryTableFieldId="2" dataDxfId="187"/>
-    <tableColumn id="3" xr3:uid="{1940D9A0-FA6D-450E-954A-327328FAD826}" uniqueName="3" name="Oszlop3" queryTableFieldId="3" dataDxfId="186"/>
-    <tableColumn id="4" xr3:uid="{2A5ED6A7-336E-4B7D-A3AC-98F46318660C}" uniqueName="4" name="Oszlop4" queryTableFieldId="4" dataDxfId="185"/>
-    <tableColumn id="5" xr3:uid="{C46B2876-075E-4A8F-9B7F-C00ED18EDD9E}" uniqueName="5" name="Oszlop5" queryTableFieldId="5" dataDxfId="184"/>
-    <tableColumn id="6" xr3:uid="{FE8BB0FA-E307-41D5-A4D5-83BC407B483B}" uniqueName="6" name="Oszlop6" queryTableFieldId="6" dataDxfId="183"/>
-    <tableColumn id="7" xr3:uid="{CF838701-4A2F-48D0-B9C6-412E40976BE5}" uniqueName="7" name="Oszlop7" queryTableFieldId="7" dataDxfId="182"/>
-    <tableColumn id="8" xr3:uid="{AD5E97A2-8DFF-4FDD-99FB-198BCC791896}" uniqueName="8" name="Oszlop8" queryTableFieldId="8" dataDxfId="181"/>
-    <tableColumn id="9" xr3:uid="{002787B7-36A3-48F0-A0FB-EAB79DED4A47}" uniqueName="9" name="Oszlop9" queryTableFieldId="9" dataDxfId="180"/>
-    <tableColumn id="10" xr3:uid="{DFC565FE-8C60-4884-8FFE-CC9333AF9395}" uniqueName="10" name="Oszlop10" queryTableFieldId="10" dataDxfId="179"/>
-    <tableColumn id="11" xr3:uid="{722E9B4E-06E4-41C4-8B7E-6FAF204EB181}" uniqueName="11" name="Oszlop11" queryTableFieldId="11" dataDxfId="178"/>
-    <tableColumn id="12" xr3:uid="{38A759ED-503A-4B6B-9F64-9079BC4F39FB}" uniqueName="12" name="Oszlop12" queryTableFieldId="12" dataDxfId="177"/>
-    <tableColumn id="13" xr3:uid="{1AC73B55-C9E0-43D0-A7BF-202C3671673B}" uniqueName="13" name="Oszlop13" queryTableFieldId="13" dataDxfId="176"/>
-    <tableColumn id="14" xr3:uid="{417BBF16-E3DA-4647-A97B-373B730DD852}" uniqueName="14" name="Oszlop14" queryTableFieldId="14" dataDxfId="175"/>
-    <tableColumn id="15" xr3:uid="{D4986906-906C-4AB4-B937-29D30057A671}" uniqueName="15" name="Oszlop15" queryTableFieldId="15" dataDxfId="174"/>
-    <tableColumn id="16" xr3:uid="{78CBD81C-A1B7-4932-B9FB-CACB8AE58870}" uniqueName="16" name="Oszlop16" queryTableFieldId="16" dataDxfId="173"/>
-    <tableColumn id="17" xr3:uid="{54C14E6E-6902-4E6B-8AE9-4B3166DB4547}" uniqueName="17" name="Oszlop17" queryTableFieldId="17" dataDxfId="172"/>
-    <tableColumn id="18" xr3:uid="{F0CF5061-6D60-476A-9917-BB304D5B2F3B}" uniqueName="18" name="Oszlop18" queryTableFieldId="18" dataDxfId="171"/>
-    <tableColumn id="19" xr3:uid="{B7ED95A7-7731-4BDD-B716-EAB0B8ADC13C}" uniqueName="19" name="Oszlop19" queryTableFieldId="19" dataDxfId="170"/>
-    <tableColumn id="20" xr3:uid="{2642BBD0-6B3B-4AC3-8E46-6AEFC98F6BF8}" uniqueName="20" name="Oszlop20" queryTableFieldId="20" dataDxfId="169"/>
-    <tableColumn id="21" xr3:uid="{A7CAB78C-7F7D-4125-8C83-844AD8BBF589}" uniqueName="21" name="Oszlop21" queryTableFieldId="21" dataDxfId="168"/>
-    <tableColumn id="22" xr3:uid="{C14EAE52-E574-4B5D-A1D3-BFD493B98DBE}" uniqueName="22" name="Oszlop22" queryTableFieldId="22" dataDxfId="167"/>
-    <tableColumn id="23" xr3:uid="{13582685-CA33-47C4-9CCB-6D9A7F52C43D}" uniqueName="23" name="Oszlop23" queryTableFieldId="23" dataDxfId="166"/>
-    <tableColumn id="24" xr3:uid="{6FFB97CC-6E70-4E82-9D90-EE0C180FBCFC}" uniqueName="24" name="Oszlop24" queryTableFieldId="24" dataDxfId="165"/>
-    <tableColumn id="25" xr3:uid="{91ED95D3-C1A0-41EB-AB8B-59048DD3F413}" uniqueName="25" name="Oszlop25" queryTableFieldId="25" dataDxfId="164"/>
-    <tableColumn id="26" xr3:uid="{A8EE2F7E-EFAB-4814-A201-71210F714BD6}" uniqueName="26" name="Oszlop26" queryTableFieldId="26" dataDxfId="163"/>
-    <tableColumn id="27" xr3:uid="{2C247694-0122-485F-9BE1-43873B9E2424}" uniqueName="27" name="Oszlop27" queryTableFieldId="27" dataDxfId="162"/>
-    <tableColumn id="28" xr3:uid="{2EC2FDCC-202F-4CF5-9841-4489828FA291}" uniqueName="28" name="Oszlop28" queryTableFieldId="28" dataDxfId="161"/>
-    <tableColumn id="29" xr3:uid="{D8947960-AC94-422C-A2E7-D39E56BDE2A4}" uniqueName="29" name="Oszlop29" queryTableFieldId="29" dataDxfId="160"/>
-    <tableColumn id="30" xr3:uid="{14352C38-138F-4075-B0CA-43086B5A7555}" uniqueName="30" name="Oszlop30" queryTableFieldId="30" dataDxfId="159"/>
-    <tableColumn id="31" xr3:uid="{EEF32F65-3DD5-4178-BE9A-871DDCA74D6C}" uniqueName="31" name="Oszlop31" queryTableFieldId="31" dataDxfId="158"/>
-    <tableColumn id="32" xr3:uid="{87798D8B-1A70-4A54-B13D-9F7FDB265EAB}" uniqueName="32" name="Oszlop32" queryTableFieldId="32" dataDxfId="157"/>
-    <tableColumn id="33" xr3:uid="{A039D294-2C3C-4282-89EC-CA945937FC89}" uniqueName="33" name="Oszlop33" queryTableFieldId="33" dataDxfId="156"/>
-    <tableColumn id="34" xr3:uid="{558BEDC9-76B9-4880-8347-5ACE25A74D4B}" uniqueName="34" name="Oszlop34" queryTableFieldId="34" dataDxfId="155"/>
-    <tableColumn id="35" xr3:uid="{32F6F95F-646E-451D-8204-1CA6125D422E}" uniqueName="35" name="Oszlop35" queryTableFieldId="35" dataDxfId="154"/>
-    <tableColumn id="36" xr3:uid="{5FA7C415-5357-44C3-8261-93E9E0756229}" uniqueName="36" name="Oszlop36" queryTableFieldId="36" dataDxfId="153"/>
-    <tableColumn id="37" xr3:uid="{D1EC40EC-AB47-4892-BC89-CE2489FCC7EC}" uniqueName="37" name="Oszlop37" queryTableFieldId="37" dataDxfId="152"/>
-    <tableColumn id="38" xr3:uid="{C660067B-ECD9-417D-8C7F-0D0FB927B147}" uniqueName="38" name="Oszlop38" queryTableFieldId="38" dataDxfId="151"/>
-    <tableColumn id="39" xr3:uid="{D8CEFF35-9BAC-4746-95F5-2FF0D0BBC54F}" uniqueName="39" name="Oszlop39" queryTableFieldId="39" dataDxfId="150"/>
-    <tableColumn id="40" xr3:uid="{94399687-0669-4E77-B1A5-0983E8273F84}" uniqueName="40" name="Oszlop40" queryTableFieldId="40" dataDxfId="149"/>
-    <tableColumn id="41" xr3:uid="{819C45A2-EFCD-43D5-AAA8-A165D044725D}" uniqueName="41" name="Oszlop41" queryTableFieldId="41" dataDxfId="148"/>
-    <tableColumn id="42" xr3:uid="{5D4F8E08-F532-4989-856B-5D53A877502A}" uniqueName="42" name="Oszlop42" queryTableFieldId="42" dataDxfId="147"/>
-    <tableColumn id="43" xr3:uid="{043A2811-1D13-4503-8E97-0ED410BEED4D}" uniqueName="43" name="Oszlop43" queryTableFieldId="43" dataDxfId="146"/>
-    <tableColumn id="44" xr3:uid="{62485A93-DE05-464F-80AD-8C33624E942A}" uniqueName="44" name="Oszlop44" queryTableFieldId="44" dataDxfId="145"/>
-    <tableColumn id="45" xr3:uid="{01708938-DD66-4F24-8BFF-0E1F1DDAD074}" uniqueName="45" name="Oszlop45" queryTableFieldId="45" dataDxfId="144"/>
-    <tableColumn id="46" xr3:uid="{3BEAEB2C-0578-4DF3-A9E0-62916847D26D}" uniqueName="46" name="Oszlop46" queryTableFieldId="46" dataDxfId="143"/>
-    <tableColumn id="47" xr3:uid="{E485321B-FF02-4BC2-AA5F-2DAF24FFB9E8}" uniqueName="47" name="Oszlop47" queryTableFieldId="47" dataDxfId="142"/>
-    <tableColumn id="48" xr3:uid="{F207BB99-37CB-4B54-923D-7608710A3094}" uniqueName="48" name="Oszlop48" queryTableFieldId="48" dataDxfId="141"/>
-    <tableColumn id="49" xr3:uid="{9C7308CF-7867-49EE-B044-C4A6A880B801}" uniqueName="49" name="Oszlop49" queryTableFieldId="49" dataDxfId="140"/>
-    <tableColumn id="50" xr3:uid="{6633743B-BD5B-4680-B85A-BEEB9268A167}" uniqueName="50" name="Oszlop50" queryTableFieldId="50" dataDxfId="139"/>
-    <tableColumn id="51" xr3:uid="{7CBC244D-621B-4B5C-BFC5-080808480784}" uniqueName="51" name="Oszlop51" queryTableFieldId="51" dataDxfId="138"/>
-    <tableColumn id="52" xr3:uid="{2672080F-A2C0-449E-B978-572D6C71ACAA}" uniqueName="52" name="Oszlop52" queryTableFieldId="52" dataDxfId="137"/>
-    <tableColumn id="53" xr3:uid="{7398282F-4BD3-4F19-80EE-83F55CD8941B}" uniqueName="53" name="Oszlop53" queryTableFieldId="53" dataDxfId="136"/>
-    <tableColumn id="54" xr3:uid="{7EC70838-1EBA-4E85-A4D1-97EAAE14C8CB}" uniqueName="54" name="Oszlop54" queryTableFieldId="54" dataDxfId="135"/>
-    <tableColumn id="55" xr3:uid="{24B25E3D-B137-4097-A429-FEF53AACE908}" uniqueName="55" name="Oszlop55" queryTableFieldId="55" dataDxfId="134"/>
-    <tableColumn id="56" xr3:uid="{E26C030B-063B-4400-B43B-DDBD3C4325FC}" uniqueName="56" name="Oszlop56" queryTableFieldId="56" dataDxfId="133"/>
-    <tableColumn id="57" xr3:uid="{F23F0C29-A916-493F-9C3A-E0522BA1C6F3}" uniqueName="57" name="Oszlop57" queryTableFieldId="57" dataDxfId="132"/>
-    <tableColumn id="58" xr3:uid="{5C492DC9-2A1E-4512-A4FA-4B5F49DB562A}" uniqueName="58" name="Oszlop58" queryTableFieldId="58" dataDxfId="131"/>
-    <tableColumn id="59" xr3:uid="{0879E9F1-DA9E-4FC9-91DD-80A87E3762FE}" uniqueName="59" name="Oszlop59" queryTableFieldId="59" dataDxfId="130"/>
-    <tableColumn id="60" xr3:uid="{DC997E2C-B6E3-43E5-8E8F-BFA01D35DAA7}" uniqueName="60" name="Oszlop60" queryTableFieldId="60" dataDxfId="129"/>
+    <tableColumn id="1" xr3:uid="{571AD5BC-C083-42BF-B574-6B0FBB157DF0}" uniqueName="1" name="Oszlop1" queryTableFieldId="1" dataDxfId="181"/>
+    <tableColumn id="2" xr3:uid="{C9DF9092-1CA9-40C8-A22F-7A8869D9424A}" uniqueName="2" name="Oszlop2" queryTableFieldId="2" dataDxfId="180"/>
+    <tableColumn id="3" xr3:uid="{1940D9A0-FA6D-450E-954A-327328FAD826}" uniqueName="3" name="Oszlop3" queryTableFieldId="3" dataDxfId="179"/>
+    <tableColumn id="4" xr3:uid="{2A5ED6A7-336E-4B7D-A3AC-98F46318660C}" uniqueName="4" name="Oszlop4" queryTableFieldId="4" dataDxfId="178"/>
+    <tableColumn id="5" xr3:uid="{C46B2876-075E-4A8F-9B7F-C00ED18EDD9E}" uniqueName="5" name="Oszlop5" queryTableFieldId="5" dataDxfId="177"/>
+    <tableColumn id="6" xr3:uid="{FE8BB0FA-E307-41D5-A4D5-83BC407B483B}" uniqueName="6" name="Oszlop6" queryTableFieldId="6" dataDxfId="176"/>
+    <tableColumn id="7" xr3:uid="{CF838701-4A2F-48D0-B9C6-412E40976BE5}" uniqueName="7" name="Oszlop7" queryTableFieldId="7" dataDxfId="175"/>
+    <tableColumn id="8" xr3:uid="{AD5E97A2-8DFF-4FDD-99FB-198BCC791896}" uniqueName="8" name="Oszlop8" queryTableFieldId="8" dataDxfId="174"/>
+    <tableColumn id="9" xr3:uid="{002787B7-36A3-48F0-A0FB-EAB79DED4A47}" uniqueName="9" name="Oszlop9" queryTableFieldId="9" dataDxfId="173"/>
+    <tableColumn id="10" xr3:uid="{DFC565FE-8C60-4884-8FFE-CC9333AF9395}" uniqueName="10" name="Oszlop10" queryTableFieldId="10" dataDxfId="172"/>
+    <tableColumn id="11" xr3:uid="{722E9B4E-06E4-41C4-8B7E-6FAF204EB181}" uniqueName="11" name="Oszlop11" queryTableFieldId="11" dataDxfId="171"/>
+    <tableColumn id="12" xr3:uid="{38A759ED-503A-4B6B-9F64-9079BC4F39FB}" uniqueName="12" name="Oszlop12" queryTableFieldId="12" dataDxfId="170"/>
+    <tableColumn id="13" xr3:uid="{1AC73B55-C9E0-43D0-A7BF-202C3671673B}" uniqueName="13" name="Oszlop13" queryTableFieldId="13" dataDxfId="169"/>
+    <tableColumn id="14" xr3:uid="{417BBF16-E3DA-4647-A97B-373B730DD852}" uniqueName="14" name="Oszlop14" queryTableFieldId="14" dataDxfId="168"/>
+    <tableColumn id="15" xr3:uid="{D4986906-906C-4AB4-B937-29D30057A671}" uniqueName="15" name="Oszlop15" queryTableFieldId="15" dataDxfId="167"/>
+    <tableColumn id="16" xr3:uid="{78CBD81C-A1B7-4932-B9FB-CACB8AE58870}" uniqueName="16" name="Oszlop16" queryTableFieldId="16" dataDxfId="166"/>
+    <tableColumn id="17" xr3:uid="{54C14E6E-6902-4E6B-8AE9-4B3166DB4547}" uniqueName="17" name="Oszlop17" queryTableFieldId="17" dataDxfId="165"/>
+    <tableColumn id="18" xr3:uid="{F0CF5061-6D60-476A-9917-BB304D5B2F3B}" uniqueName="18" name="Oszlop18" queryTableFieldId="18" dataDxfId="164"/>
+    <tableColumn id="19" xr3:uid="{B7ED95A7-7731-4BDD-B716-EAB0B8ADC13C}" uniqueName="19" name="Oszlop19" queryTableFieldId="19" dataDxfId="163"/>
+    <tableColumn id="20" xr3:uid="{2642BBD0-6B3B-4AC3-8E46-6AEFC98F6BF8}" uniqueName="20" name="Oszlop20" queryTableFieldId="20" dataDxfId="162"/>
+    <tableColumn id="21" xr3:uid="{A7CAB78C-7F7D-4125-8C83-844AD8BBF589}" uniqueName="21" name="Oszlop21" queryTableFieldId="21" dataDxfId="161"/>
+    <tableColumn id="22" xr3:uid="{C14EAE52-E574-4B5D-A1D3-BFD493B98DBE}" uniqueName="22" name="Oszlop22" queryTableFieldId="22" dataDxfId="160"/>
+    <tableColumn id="23" xr3:uid="{13582685-CA33-47C4-9CCB-6D9A7F52C43D}" uniqueName="23" name="Oszlop23" queryTableFieldId="23" dataDxfId="159"/>
+    <tableColumn id="24" xr3:uid="{6FFB97CC-6E70-4E82-9D90-EE0C180FBCFC}" uniqueName="24" name="Oszlop24" queryTableFieldId="24" dataDxfId="158"/>
+    <tableColumn id="25" xr3:uid="{91ED95D3-C1A0-41EB-AB8B-59048DD3F413}" uniqueName="25" name="Oszlop25" queryTableFieldId="25" dataDxfId="157"/>
+    <tableColumn id="26" xr3:uid="{A8EE2F7E-EFAB-4814-A201-71210F714BD6}" uniqueName="26" name="Oszlop26" queryTableFieldId="26" dataDxfId="156"/>
+    <tableColumn id="27" xr3:uid="{2C247694-0122-485F-9BE1-43873B9E2424}" uniqueName="27" name="Oszlop27" queryTableFieldId="27" dataDxfId="155"/>
+    <tableColumn id="28" xr3:uid="{2EC2FDCC-202F-4CF5-9841-4489828FA291}" uniqueName="28" name="Oszlop28" queryTableFieldId="28" dataDxfId="154"/>
+    <tableColumn id="29" xr3:uid="{D8947960-AC94-422C-A2E7-D39E56BDE2A4}" uniqueName="29" name="Oszlop29" queryTableFieldId="29" dataDxfId="153"/>
+    <tableColumn id="30" xr3:uid="{14352C38-138F-4075-B0CA-43086B5A7555}" uniqueName="30" name="Oszlop30" queryTableFieldId="30" dataDxfId="152"/>
+    <tableColumn id="31" xr3:uid="{EEF32F65-3DD5-4178-BE9A-871DDCA74D6C}" uniqueName="31" name="Oszlop31" queryTableFieldId="31" dataDxfId="151"/>
+    <tableColumn id="32" xr3:uid="{87798D8B-1A70-4A54-B13D-9F7FDB265EAB}" uniqueName="32" name="Oszlop32" queryTableFieldId="32" dataDxfId="150"/>
+    <tableColumn id="33" xr3:uid="{A039D294-2C3C-4282-89EC-CA945937FC89}" uniqueName="33" name="Oszlop33" queryTableFieldId="33" dataDxfId="149"/>
+    <tableColumn id="34" xr3:uid="{558BEDC9-76B9-4880-8347-5ACE25A74D4B}" uniqueName="34" name="Oszlop34" queryTableFieldId="34" dataDxfId="148"/>
+    <tableColumn id="35" xr3:uid="{32F6F95F-646E-451D-8204-1CA6125D422E}" uniqueName="35" name="Oszlop35" queryTableFieldId="35" dataDxfId="147"/>
+    <tableColumn id="36" xr3:uid="{5FA7C415-5357-44C3-8261-93E9E0756229}" uniqueName="36" name="Oszlop36" queryTableFieldId="36" dataDxfId="146"/>
+    <tableColumn id="37" xr3:uid="{D1EC40EC-AB47-4892-BC89-CE2489FCC7EC}" uniqueName="37" name="Oszlop37" queryTableFieldId="37" dataDxfId="145"/>
+    <tableColumn id="38" xr3:uid="{C660067B-ECD9-417D-8C7F-0D0FB927B147}" uniqueName="38" name="Oszlop38" queryTableFieldId="38" dataDxfId="144"/>
+    <tableColumn id="39" xr3:uid="{D8CEFF35-9BAC-4746-95F5-2FF0D0BBC54F}" uniqueName="39" name="Oszlop39" queryTableFieldId="39" dataDxfId="143"/>
+    <tableColumn id="40" xr3:uid="{94399687-0669-4E77-B1A5-0983E8273F84}" uniqueName="40" name="Oszlop40" queryTableFieldId="40" dataDxfId="142"/>
+    <tableColumn id="41" xr3:uid="{819C45A2-EFCD-43D5-AAA8-A165D044725D}" uniqueName="41" name="Oszlop41" queryTableFieldId="41" dataDxfId="141"/>
+    <tableColumn id="42" xr3:uid="{5D4F8E08-F532-4989-856B-5D53A877502A}" uniqueName="42" name="Oszlop42" queryTableFieldId="42" dataDxfId="140"/>
+    <tableColumn id="43" xr3:uid="{043A2811-1D13-4503-8E97-0ED410BEED4D}" uniqueName="43" name="Oszlop43" queryTableFieldId="43" dataDxfId="139"/>
+    <tableColumn id="44" xr3:uid="{62485A93-DE05-464F-80AD-8C33624E942A}" uniqueName="44" name="Oszlop44" queryTableFieldId="44" dataDxfId="138"/>
+    <tableColumn id="45" xr3:uid="{01708938-DD66-4F24-8BFF-0E1F1DDAD074}" uniqueName="45" name="Oszlop45" queryTableFieldId="45" dataDxfId="137"/>
+    <tableColumn id="46" xr3:uid="{3BEAEB2C-0578-4DF3-A9E0-62916847D26D}" uniqueName="46" name="Oszlop46" queryTableFieldId="46" dataDxfId="136"/>
+    <tableColumn id="47" xr3:uid="{E485321B-FF02-4BC2-AA5F-2DAF24FFB9E8}" uniqueName="47" name="Oszlop47" queryTableFieldId="47" dataDxfId="135"/>
+    <tableColumn id="48" xr3:uid="{F207BB99-37CB-4B54-923D-7608710A3094}" uniqueName="48" name="Oszlop48" queryTableFieldId="48" dataDxfId="134"/>
+    <tableColumn id="49" xr3:uid="{9C7308CF-7867-49EE-B044-C4A6A880B801}" uniqueName="49" name="Oszlop49" queryTableFieldId="49" dataDxfId="133"/>
+    <tableColumn id="50" xr3:uid="{6633743B-BD5B-4680-B85A-BEEB9268A167}" uniqueName="50" name="Oszlop50" queryTableFieldId="50" dataDxfId="132"/>
+    <tableColumn id="51" xr3:uid="{7CBC244D-621B-4B5C-BFC5-080808480784}" uniqueName="51" name="Oszlop51" queryTableFieldId="51" dataDxfId="131"/>
+    <tableColumn id="52" xr3:uid="{2672080F-A2C0-449E-B978-572D6C71ACAA}" uniqueName="52" name="Oszlop52" queryTableFieldId="52" dataDxfId="130"/>
+    <tableColumn id="53" xr3:uid="{7398282F-4BD3-4F19-80EE-83F55CD8941B}" uniqueName="53" name="Oszlop53" queryTableFieldId="53" dataDxfId="129"/>
+    <tableColumn id="54" xr3:uid="{7EC70838-1EBA-4E85-A4D1-97EAAE14C8CB}" uniqueName="54" name="Oszlop54" queryTableFieldId="54" dataDxfId="128"/>
+    <tableColumn id="55" xr3:uid="{24B25E3D-B137-4097-A429-FEF53AACE908}" uniqueName="55" name="Oszlop55" queryTableFieldId="55" dataDxfId="127"/>
+    <tableColumn id="56" xr3:uid="{E26C030B-063B-4400-B43B-DDBD3C4325FC}" uniqueName="56" name="Oszlop56" queryTableFieldId="56" dataDxfId="126"/>
+    <tableColumn id="57" xr3:uid="{F23F0C29-A916-493F-9C3A-E0522BA1C6F3}" uniqueName="57" name="Oszlop57" queryTableFieldId="57" dataDxfId="125"/>
+    <tableColumn id="58" xr3:uid="{5C492DC9-2A1E-4512-A4FA-4B5F49DB562A}" uniqueName="58" name="Oszlop58" queryTableFieldId="58" dataDxfId="124"/>
+    <tableColumn id="59" xr3:uid="{0879E9F1-DA9E-4FC9-91DD-80A87E3762FE}" uniqueName="59" name="Oszlop59" queryTableFieldId="59" dataDxfId="123"/>
+    <tableColumn id="60" xr3:uid="{DC997E2C-B6E3-43E5-8E8F-BFA01D35DAA7}" uniqueName="60" name="Oszlop60" queryTableFieldId="60" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1484,66 +1483,66 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C07AE6A8-E806-4BB7-97F9-5DB367900E0A}" name="Új_szöveges_dokumentum__3" displayName="Új_szöveges_dokumentum__3" ref="A1:BH61" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:BH61" xr:uid="{D9770763-7B96-40ED-9684-67C21BAADD58}"/>
   <tableColumns count="60">
-    <tableColumn id="1" xr3:uid="{0648BDF8-8B06-403E-9E86-5D2F32837592}" uniqueName="1" name="Column1.1" queryTableFieldId="1" dataDxfId="128"/>
-    <tableColumn id="2" xr3:uid="{84D15E2F-094F-4135-B5A5-80F9B3EBEA91}" uniqueName="2" name="Column1.2" queryTableFieldId="2" dataDxfId="127"/>
-    <tableColumn id="3" xr3:uid="{E437536C-33D7-437A-A5DE-3AD0BB8530AA}" uniqueName="3" name="Column1.3" queryTableFieldId="3" dataDxfId="126"/>
-    <tableColumn id="4" xr3:uid="{2F5366DC-2A0A-4B28-A1D3-89537D16F995}" uniqueName="4" name="Column1.4" queryTableFieldId="4" dataDxfId="125"/>
-    <tableColumn id="5" xr3:uid="{CB98375A-B6D8-4AA3-A46E-2F49262822FF}" uniqueName="5" name="Column1.5" queryTableFieldId="5" dataDxfId="124"/>
-    <tableColumn id="6" xr3:uid="{E541345A-AB87-4B41-87DD-C7194670F815}" uniqueName="6" name="Column1.6" queryTableFieldId="6" dataDxfId="123"/>
-    <tableColumn id="7" xr3:uid="{C9184BF0-FC95-4599-8958-1B22876DC7B4}" uniqueName="7" name="Column1.7" queryTableFieldId="7" dataDxfId="122"/>
-    <tableColumn id="8" xr3:uid="{126302AA-E12D-4D59-A53A-7608B1EE67A2}" uniqueName="8" name="Column1.8" queryTableFieldId="8" dataDxfId="121"/>
-    <tableColumn id="9" xr3:uid="{82AB11A2-C54B-4CE9-83CE-D42C4D4129B2}" uniqueName="9" name="Column1.9" queryTableFieldId="9" dataDxfId="120"/>
-    <tableColumn id="10" xr3:uid="{9315561E-349F-48AD-8315-F59708CE8A03}" uniqueName="10" name="Column1.10" queryTableFieldId="10" dataDxfId="119"/>
-    <tableColumn id="11" xr3:uid="{C17B3442-7F2A-40D4-9546-A76AD6454B67}" uniqueName="11" name="Column1.11" queryTableFieldId="11" dataDxfId="118"/>
-    <tableColumn id="12" xr3:uid="{AFBDEFDE-87DA-4B8A-A818-3197AD975332}" uniqueName="12" name="Column1.12" queryTableFieldId="12" dataDxfId="117"/>
-    <tableColumn id="13" xr3:uid="{F0CFFB68-497F-4197-9448-C89F5D611672}" uniqueName="13" name="Column1.13" queryTableFieldId="13" dataDxfId="116"/>
-    <tableColumn id="14" xr3:uid="{3A43F006-088A-477A-8655-BAA94734456B}" uniqueName="14" name="Column1.14" queryTableFieldId="14" dataDxfId="115"/>
-    <tableColumn id="15" xr3:uid="{77EA3E2F-B905-4C01-9553-D2F78EEB7A9A}" uniqueName="15" name="Column1.15" queryTableFieldId="15" dataDxfId="114"/>
-    <tableColumn id="16" xr3:uid="{8B3F1F08-1C80-4278-BFE9-B8D034ABBCE8}" uniqueName="16" name="Column1.16" queryTableFieldId="16" dataDxfId="113"/>
-    <tableColumn id="17" xr3:uid="{49BB1F56-590B-4A81-A3FE-1DD26DAEF76D}" uniqueName="17" name="Column1.17" queryTableFieldId="17" dataDxfId="112"/>
-    <tableColumn id="18" xr3:uid="{E95D779D-48ED-4FBF-BE8D-74C6B0E1D0DD}" uniqueName="18" name="Column1.18" queryTableFieldId="18" dataDxfId="111"/>
-    <tableColumn id="19" xr3:uid="{F0D6981F-ABBD-431A-93B3-DB449292A434}" uniqueName="19" name="Column1.19" queryTableFieldId="19" dataDxfId="110"/>
-    <tableColumn id="20" xr3:uid="{5FE35A7B-7F5E-4024-AAE7-7A91242BB0E2}" uniqueName="20" name="Column1.20" queryTableFieldId="20" dataDxfId="109"/>
-    <tableColumn id="21" xr3:uid="{4824657C-B901-4457-9D71-BE8545BFF59E}" uniqueName="21" name="Column1.21" queryTableFieldId="21" dataDxfId="108"/>
-    <tableColumn id="22" xr3:uid="{0F76AE10-7990-4646-9063-7CB5927CF57D}" uniqueName="22" name="Column1.22" queryTableFieldId="22" dataDxfId="107"/>
-    <tableColumn id="23" xr3:uid="{CDE05BA2-0168-4037-BBCB-E7E43C25BC07}" uniqueName="23" name="Column1.23" queryTableFieldId="23" dataDxfId="106"/>
-    <tableColumn id="24" xr3:uid="{540AD185-AD46-4276-A676-176B3C80437C}" uniqueName="24" name="Column1.24" queryTableFieldId="24" dataDxfId="105"/>
-    <tableColumn id="25" xr3:uid="{234C3E50-7BD9-4707-9F14-E4DB15EDBDDC}" uniqueName="25" name="Column1.25" queryTableFieldId="25" dataDxfId="104"/>
-    <tableColumn id="26" xr3:uid="{8A2E9515-D4E6-46B5-8B8B-64A789C08B20}" uniqueName="26" name="Column1.26" queryTableFieldId="26" dataDxfId="103"/>
-    <tableColumn id="27" xr3:uid="{6FBE3FD3-5E57-4848-9D44-B0F71A36FF5D}" uniqueName="27" name="Column1.27" queryTableFieldId="27" dataDxfId="102"/>
-    <tableColumn id="28" xr3:uid="{2802380B-97A7-4248-9D46-E8C71BFB6561}" uniqueName="28" name="Column1.28" queryTableFieldId="28" dataDxfId="101"/>
-    <tableColumn id="29" xr3:uid="{75FA5252-D8FF-4F73-9DAF-42C55D8C6373}" uniqueName="29" name="Column1.29" queryTableFieldId="29" dataDxfId="100"/>
-    <tableColumn id="30" xr3:uid="{9616F543-C9FC-4532-86E4-14899C58050A}" uniqueName="30" name="Column1.30" queryTableFieldId="30" dataDxfId="99"/>
-    <tableColumn id="31" xr3:uid="{C1D709BB-C5DD-4357-9C81-75C75E1B3B97}" uniqueName="31" name="Column1.31" queryTableFieldId="31" dataDxfId="98"/>
-    <tableColumn id="32" xr3:uid="{899049E1-3B00-4B87-BFD7-BFE13E568A70}" uniqueName="32" name="Column1.32" queryTableFieldId="32" dataDxfId="97"/>
-    <tableColumn id="33" xr3:uid="{1ED84722-061C-48E3-A05E-2E55BB561EB9}" uniqueName="33" name="Column1.33" queryTableFieldId="33" dataDxfId="96"/>
-    <tableColumn id="34" xr3:uid="{829B33CA-1819-47D4-A2CF-E07AC6B66D53}" uniqueName="34" name="Column1.34" queryTableFieldId="34" dataDxfId="95"/>
-    <tableColumn id="35" xr3:uid="{B4980626-4D5B-482C-B07F-A93C1F230C06}" uniqueName="35" name="Column1.35" queryTableFieldId="35" dataDxfId="94"/>
-    <tableColumn id="36" xr3:uid="{3050A5F7-901A-4FEF-97F1-965B3605E2B3}" uniqueName="36" name="Column1.36" queryTableFieldId="36" dataDxfId="93"/>
-    <tableColumn id="37" xr3:uid="{4F68D6FA-FB59-4FF6-BA25-4B3984FB25AE}" uniqueName="37" name="Column1.37" queryTableFieldId="37" dataDxfId="92"/>
-    <tableColumn id="38" xr3:uid="{F273478B-1438-40A6-AC68-50F57E2D5718}" uniqueName="38" name="Column1.38" queryTableFieldId="38" dataDxfId="91"/>
-    <tableColumn id="39" xr3:uid="{CD6C5582-611A-40BD-B833-A0B3E57A74CA}" uniqueName="39" name="Column1.39" queryTableFieldId="39" dataDxfId="90"/>
-    <tableColumn id="40" xr3:uid="{7343C076-C27C-4644-AE85-9F6FC922D2B0}" uniqueName="40" name="Column1.40" queryTableFieldId="40" dataDxfId="89"/>
-    <tableColumn id="41" xr3:uid="{DB9F0D05-3534-4DDA-8B12-1864A40840A0}" uniqueName="41" name="Column1.41" queryTableFieldId="41" dataDxfId="88"/>
-    <tableColumn id="42" xr3:uid="{3DD0491C-8A69-4508-96E7-C597EF3554D7}" uniqueName="42" name="Column1.42" queryTableFieldId="42" dataDxfId="87"/>
-    <tableColumn id="43" xr3:uid="{87F65035-7009-4AB3-8655-DD918C6955F6}" uniqueName="43" name="Column1.43" queryTableFieldId="43" dataDxfId="86"/>
-    <tableColumn id="44" xr3:uid="{36797F7C-B360-4ECE-8C0F-BD67D65840D6}" uniqueName="44" name="Column1.44" queryTableFieldId="44" dataDxfId="85"/>
-    <tableColumn id="45" xr3:uid="{669B14B5-7E3C-48DE-A1CF-719B74067FF8}" uniqueName="45" name="Column1.45" queryTableFieldId="45" dataDxfId="84"/>
-    <tableColumn id="46" xr3:uid="{71601A84-A2FC-45C6-A105-6AC6DC771181}" uniqueName="46" name="Column1.46" queryTableFieldId="46" dataDxfId="83"/>
-    <tableColumn id="47" xr3:uid="{A3249BC4-6EFF-424E-B9D5-5D8715A4AD60}" uniqueName="47" name="Column1.47" queryTableFieldId="47" dataDxfId="82"/>
-    <tableColumn id="48" xr3:uid="{988633E5-F147-4522-93AE-EEAA17E9467D}" uniqueName="48" name="Column1.48" queryTableFieldId="48" dataDxfId="81"/>
-    <tableColumn id="49" xr3:uid="{9CD0C380-8831-4744-847E-A1945E7229FC}" uniqueName="49" name="Column1.49" queryTableFieldId="49" dataDxfId="80"/>
-    <tableColumn id="50" xr3:uid="{EC3F6160-105C-4FBA-A931-247F8B5FD1FD}" uniqueName="50" name="Column1.50" queryTableFieldId="50" dataDxfId="79"/>
-    <tableColumn id="51" xr3:uid="{343244BA-2B5A-482C-BC9E-0B898E8B7DE7}" uniqueName="51" name="Column1.51" queryTableFieldId="51" dataDxfId="78"/>
-    <tableColumn id="52" xr3:uid="{5D3B022D-7C17-49E6-B70B-D182B053C165}" uniqueName="52" name="Column1.52" queryTableFieldId="52" dataDxfId="77"/>
-    <tableColumn id="53" xr3:uid="{869DCAC3-106C-4505-9310-F5BB01987287}" uniqueName="53" name="Column1.53" queryTableFieldId="53" dataDxfId="76"/>
-    <tableColumn id="54" xr3:uid="{37B3D497-8231-4B91-8B91-70A961B538E1}" uniqueName="54" name="Column1.54" queryTableFieldId="54" dataDxfId="75"/>
-    <tableColumn id="55" xr3:uid="{15787987-2B12-4E6A-8F6A-9C2549BCE16E}" uniqueName="55" name="Column1.55" queryTableFieldId="55" dataDxfId="74"/>
-    <tableColumn id="56" xr3:uid="{C4A39D23-4333-4912-BF82-803C2E263EA4}" uniqueName="56" name="Column1.56" queryTableFieldId="56" dataDxfId="73"/>
-    <tableColumn id="57" xr3:uid="{BE3F2F0D-13BC-4368-A1B0-063FEAED7968}" uniqueName="57" name="Column1.57" queryTableFieldId="57" dataDxfId="72"/>
-    <tableColumn id="58" xr3:uid="{6FF92256-B3D1-409E-A082-8963B50A3EFA}" uniqueName="58" name="Column1.58" queryTableFieldId="58" dataDxfId="71"/>
-    <tableColumn id="59" xr3:uid="{F700ACA9-09F3-486A-AA4B-0D412A322362}" uniqueName="59" name="Column1.59" queryTableFieldId="59" dataDxfId="70"/>
-    <tableColumn id="60" xr3:uid="{B2A3C236-FE0C-40D2-87DE-515C4EB20572}" uniqueName="60" name="Column1.60" queryTableFieldId="60" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{0648BDF8-8B06-403E-9E86-5D2F32837592}" uniqueName="1" name="Column1.1" queryTableFieldId="1" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{84D15E2F-094F-4135-B5A5-80F9B3EBEA91}" uniqueName="2" name="Column1.2" queryTableFieldId="2" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{E437536C-33D7-437A-A5DE-3AD0BB8530AA}" uniqueName="3" name="Column1.3" queryTableFieldId="3" dataDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{2F5366DC-2A0A-4B28-A1D3-89537D16F995}" uniqueName="4" name="Column1.4" queryTableFieldId="4" dataDxfId="118"/>
+    <tableColumn id="5" xr3:uid="{CB98375A-B6D8-4AA3-A46E-2F49262822FF}" uniqueName="5" name="Column1.5" queryTableFieldId="5" dataDxfId="117"/>
+    <tableColumn id="6" xr3:uid="{E541345A-AB87-4B41-87DD-C7194670F815}" uniqueName="6" name="Column1.6" queryTableFieldId="6" dataDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{C9184BF0-FC95-4599-8958-1B22876DC7B4}" uniqueName="7" name="Column1.7" queryTableFieldId="7" dataDxfId="115"/>
+    <tableColumn id="8" xr3:uid="{126302AA-E12D-4D59-A53A-7608B1EE67A2}" uniqueName="8" name="Column1.8" queryTableFieldId="8" dataDxfId="114"/>
+    <tableColumn id="9" xr3:uid="{82AB11A2-C54B-4CE9-83CE-D42C4D4129B2}" uniqueName="9" name="Column1.9" queryTableFieldId="9" dataDxfId="113"/>
+    <tableColumn id="10" xr3:uid="{9315561E-349F-48AD-8315-F59708CE8A03}" uniqueName="10" name="Column1.10" queryTableFieldId="10" dataDxfId="112"/>
+    <tableColumn id="11" xr3:uid="{C17B3442-7F2A-40D4-9546-A76AD6454B67}" uniqueName="11" name="Column1.11" queryTableFieldId="11" dataDxfId="111"/>
+    <tableColumn id="12" xr3:uid="{AFBDEFDE-87DA-4B8A-A818-3197AD975332}" uniqueName="12" name="Column1.12" queryTableFieldId="12" dataDxfId="110"/>
+    <tableColumn id="13" xr3:uid="{F0CFFB68-497F-4197-9448-C89F5D611672}" uniqueName="13" name="Column1.13" queryTableFieldId="13" dataDxfId="109"/>
+    <tableColumn id="14" xr3:uid="{3A43F006-088A-477A-8655-BAA94734456B}" uniqueName="14" name="Column1.14" queryTableFieldId="14" dataDxfId="108"/>
+    <tableColumn id="15" xr3:uid="{77EA3E2F-B905-4C01-9553-D2F78EEB7A9A}" uniqueName="15" name="Column1.15" queryTableFieldId="15" dataDxfId="107"/>
+    <tableColumn id="16" xr3:uid="{8B3F1F08-1C80-4278-BFE9-B8D034ABBCE8}" uniqueName="16" name="Column1.16" queryTableFieldId="16" dataDxfId="106"/>
+    <tableColumn id="17" xr3:uid="{49BB1F56-590B-4A81-A3FE-1DD26DAEF76D}" uniqueName="17" name="Column1.17" queryTableFieldId="17" dataDxfId="105"/>
+    <tableColumn id="18" xr3:uid="{E95D779D-48ED-4FBF-BE8D-74C6B0E1D0DD}" uniqueName="18" name="Column1.18" queryTableFieldId="18" dataDxfId="104"/>
+    <tableColumn id="19" xr3:uid="{F0D6981F-ABBD-431A-93B3-DB449292A434}" uniqueName="19" name="Column1.19" queryTableFieldId="19" dataDxfId="103"/>
+    <tableColumn id="20" xr3:uid="{5FE35A7B-7F5E-4024-AAE7-7A91242BB0E2}" uniqueName="20" name="Column1.20" queryTableFieldId="20" dataDxfId="102"/>
+    <tableColumn id="21" xr3:uid="{4824657C-B901-4457-9D71-BE8545BFF59E}" uniqueName="21" name="Column1.21" queryTableFieldId="21" dataDxfId="101"/>
+    <tableColumn id="22" xr3:uid="{0F76AE10-7990-4646-9063-7CB5927CF57D}" uniqueName="22" name="Column1.22" queryTableFieldId="22" dataDxfId="100"/>
+    <tableColumn id="23" xr3:uid="{CDE05BA2-0168-4037-BBCB-E7E43C25BC07}" uniqueName="23" name="Column1.23" queryTableFieldId="23" dataDxfId="99"/>
+    <tableColumn id="24" xr3:uid="{540AD185-AD46-4276-A676-176B3C80437C}" uniqueName="24" name="Column1.24" queryTableFieldId="24" dataDxfId="98"/>
+    <tableColumn id="25" xr3:uid="{234C3E50-7BD9-4707-9F14-E4DB15EDBDDC}" uniqueName="25" name="Column1.25" queryTableFieldId="25" dataDxfId="97"/>
+    <tableColumn id="26" xr3:uid="{8A2E9515-D4E6-46B5-8B8B-64A789C08B20}" uniqueName="26" name="Column1.26" queryTableFieldId="26" dataDxfId="96"/>
+    <tableColumn id="27" xr3:uid="{6FBE3FD3-5E57-4848-9D44-B0F71A36FF5D}" uniqueName="27" name="Column1.27" queryTableFieldId="27" dataDxfId="95"/>
+    <tableColumn id="28" xr3:uid="{2802380B-97A7-4248-9D46-E8C71BFB6561}" uniqueName="28" name="Column1.28" queryTableFieldId="28" dataDxfId="94"/>
+    <tableColumn id="29" xr3:uid="{75FA5252-D8FF-4F73-9DAF-42C55D8C6373}" uniqueName="29" name="Column1.29" queryTableFieldId="29" dataDxfId="93"/>
+    <tableColumn id="30" xr3:uid="{9616F543-C9FC-4532-86E4-14899C58050A}" uniqueName="30" name="Column1.30" queryTableFieldId="30" dataDxfId="92"/>
+    <tableColumn id="31" xr3:uid="{C1D709BB-C5DD-4357-9C81-75C75E1B3B97}" uniqueName="31" name="Column1.31" queryTableFieldId="31" dataDxfId="91"/>
+    <tableColumn id="32" xr3:uid="{899049E1-3B00-4B87-BFD7-BFE13E568A70}" uniqueName="32" name="Column1.32" queryTableFieldId="32" dataDxfId="90"/>
+    <tableColumn id="33" xr3:uid="{1ED84722-061C-48E3-A05E-2E55BB561EB9}" uniqueName="33" name="Column1.33" queryTableFieldId="33" dataDxfId="89"/>
+    <tableColumn id="34" xr3:uid="{829B33CA-1819-47D4-A2CF-E07AC6B66D53}" uniqueName="34" name="Column1.34" queryTableFieldId="34" dataDxfId="88"/>
+    <tableColumn id="35" xr3:uid="{B4980626-4D5B-482C-B07F-A93C1F230C06}" uniqueName="35" name="Column1.35" queryTableFieldId="35" dataDxfId="87"/>
+    <tableColumn id="36" xr3:uid="{3050A5F7-901A-4FEF-97F1-965B3605E2B3}" uniqueName="36" name="Column1.36" queryTableFieldId="36" dataDxfId="86"/>
+    <tableColumn id="37" xr3:uid="{4F68D6FA-FB59-4FF6-BA25-4B3984FB25AE}" uniqueName="37" name="Column1.37" queryTableFieldId="37" dataDxfId="85"/>
+    <tableColumn id="38" xr3:uid="{F273478B-1438-40A6-AC68-50F57E2D5718}" uniqueName="38" name="Column1.38" queryTableFieldId="38" dataDxfId="84"/>
+    <tableColumn id="39" xr3:uid="{CD6C5582-611A-40BD-B833-A0B3E57A74CA}" uniqueName="39" name="Column1.39" queryTableFieldId="39" dataDxfId="83"/>
+    <tableColumn id="40" xr3:uid="{7343C076-C27C-4644-AE85-9F6FC922D2B0}" uniqueName="40" name="Column1.40" queryTableFieldId="40" dataDxfId="82"/>
+    <tableColumn id="41" xr3:uid="{DB9F0D05-3534-4DDA-8B12-1864A40840A0}" uniqueName="41" name="Column1.41" queryTableFieldId="41" dataDxfId="81"/>
+    <tableColumn id="42" xr3:uid="{3DD0491C-8A69-4508-96E7-C597EF3554D7}" uniqueName="42" name="Column1.42" queryTableFieldId="42" dataDxfId="80"/>
+    <tableColumn id="43" xr3:uid="{87F65035-7009-4AB3-8655-DD918C6955F6}" uniqueName="43" name="Column1.43" queryTableFieldId="43" dataDxfId="79"/>
+    <tableColumn id="44" xr3:uid="{36797F7C-B360-4ECE-8C0F-BD67D65840D6}" uniqueName="44" name="Column1.44" queryTableFieldId="44" dataDxfId="78"/>
+    <tableColumn id="45" xr3:uid="{669B14B5-7E3C-48DE-A1CF-719B74067FF8}" uniqueName="45" name="Column1.45" queryTableFieldId="45" dataDxfId="77"/>
+    <tableColumn id="46" xr3:uid="{71601A84-A2FC-45C6-A105-6AC6DC771181}" uniqueName="46" name="Column1.46" queryTableFieldId="46" dataDxfId="76"/>
+    <tableColumn id="47" xr3:uid="{A3249BC4-6EFF-424E-B9D5-5D8715A4AD60}" uniqueName="47" name="Column1.47" queryTableFieldId="47" dataDxfId="75"/>
+    <tableColumn id="48" xr3:uid="{988633E5-F147-4522-93AE-EEAA17E9467D}" uniqueName="48" name="Column1.48" queryTableFieldId="48" dataDxfId="74"/>
+    <tableColumn id="49" xr3:uid="{9CD0C380-8831-4744-847E-A1945E7229FC}" uniqueName="49" name="Column1.49" queryTableFieldId="49" dataDxfId="73"/>
+    <tableColumn id="50" xr3:uid="{EC3F6160-105C-4FBA-A931-247F8B5FD1FD}" uniqueName="50" name="Column1.50" queryTableFieldId="50" dataDxfId="72"/>
+    <tableColumn id="51" xr3:uid="{343244BA-2B5A-482C-BC9E-0B898E8B7DE7}" uniqueName="51" name="Column1.51" queryTableFieldId="51" dataDxfId="71"/>
+    <tableColumn id="52" xr3:uid="{5D3B022D-7C17-49E6-B70B-D182B053C165}" uniqueName="52" name="Column1.52" queryTableFieldId="52" dataDxfId="70"/>
+    <tableColumn id="53" xr3:uid="{869DCAC3-106C-4505-9310-F5BB01987287}" uniqueName="53" name="Column1.53" queryTableFieldId="53" dataDxfId="69"/>
+    <tableColumn id="54" xr3:uid="{37B3D497-8231-4B91-8B91-70A961B538E1}" uniqueName="54" name="Column1.54" queryTableFieldId="54" dataDxfId="68"/>
+    <tableColumn id="55" xr3:uid="{15787987-2B12-4E6A-8F6A-9C2549BCE16E}" uniqueName="55" name="Column1.55" queryTableFieldId="55" dataDxfId="67"/>
+    <tableColumn id="56" xr3:uid="{C4A39D23-4333-4912-BF82-803C2E263EA4}" uniqueName="56" name="Column1.56" queryTableFieldId="56" dataDxfId="66"/>
+    <tableColumn id="57" xr3:uid="{BE3F2F0D-13BC-4368-A1B0-063FEAED7968}" uniqueName="57" name="Column1.57" queryTableFieldId="57" dataDxfId="65"/>
+    <tableColumn id="58" xr3:uid="{6FF92256-B3D1-409E-A082-8963B50A3EFA}" uniqueName="58" name="Column1.58" queryTableFieldId="58" dataDxfId="64"/>
+    <tableColumn id="59" xr3:uid="{F700ACA9-09F3-486A-AA4B-0D412A322362}" uniqueName="59" name="Column1.59" queryTableFieldId="59" dataDxfId="63"/>
+    <tableColumn id="60" xr3:uid="{B2A3C236-FE0C-40D2-87DE-515C4EB20572}" uniqueName="60" name="Column1.60" queryTableFieldId="60" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1553,68 +1552,68 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{56AC44DD-69C9-4C9D-99ED-DF2DB7A6AF29}" name="new_1" displayName="new_1" ref="A1:BJ3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:BJ3" xr:uid="{03D2B6C6-6DD2-432D-A411-E9479FC03544}"/>
   <tableColumns count="62">
-    <tableColumn id="1" xr3:uid="{98D7E3A4-39DE-47DA-B944-49F0A0557E5E}" uniqueName="1" name="Column1.1" queryTableFieldId="1" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{509FB6ED-99F2-4BA7-88F1-D89840A7811D}" uniqueName="2" name="Column1.2" queryTableFieldId="2" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{419A591C-63BF-414F-BA41-385855C462C5}" uniqueName="3" name="Column1.3" queryTableFieldId="3" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{314CDC71-6274-4F19-B9F7-6415F8BA4687}" uniqueName="4" name="Column1.4" queryTableFieldId="4" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{6833C0D6-8864-420C-BE0E-1074B5CC7001}" uniqueName="5" name="Column1.5" queryTableFieldId="5" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{500A35EC-ECFA-4C32-A548-3FCC313C4F84}" uniqueName="6" name="Column1.6" queryTableFieldId="6" dataDxfId="63"/>
-    <tableColumn id="7" xr3:uid="{B3D8B8ED-1C0E-4F03-9ECB-9AC46B3CD351}" uniqueName="7" name="Column1.7" queryTableFieldId="7" dataDxfId="62"/>
-    <tableColumn id="8" xr3:uid="{CBCC21E0-9F71-40A0-AEAA-592F841E8838}" uniqueName="8" name="Column1.8" queryTableFieldId="8" dataDxfId="61"/>
-    <tableColumn id="9" xr3:uid="{54B3DF67-DE7B-4698-A77F-9B809ABF105F}" uniqueName="9" name="Column1.9" queryTableFieldId="9" dataDxfId="60"/>
-    <tableColumn id="10" xr3:uid="{1F4B4B60-7C8A-4787-93DA-BEA5BCBC30E0}" uniqueName="10" name="Column1.10" queryTableFieldId="10" dataDxfId="59"/>
-    <tableColumn id="11" xr3:uid="{B8AF0B34-E3D2-448B-99BE-4BA87ECF720C}" uniqueName="11" name="Column1.11" queryTableFieldId="11" dataDxfId="58"/>
-    <tableColumn id="12" xr3:uid="{BAABB28F-07F3-43A6-95AF-5AE4E22ADFC3}" uniqueName="12" name="Column1.12" queryTableFieldId="12" dataDxfId="57"/>
-    <tableColumn id="13" xr3:uid="{6519F06B-2422-425E-8296-23A84F1F2FFE}" uniqueName="13" name="Column1.13" queryTableFieldId="13" dataDxfId="56"/>
-    <tableColumn id="14" xr3:uid="{2CB1F290-4BBD-4E61-B61D-46BDB8CE41FA}" uniqueName="14" name="Column1.14" queryTableFieldId="14" dataDxfId="55"/>
-    <tableColumn id="15" xr3:uid="{74E4D9B8-6A6C-45A1-BECA-E84B35CD2549}" uniqueName="15" name="Column1.15" queryTableFieldId="15" dataDxfId="54"/>
-    <tableColumn id="16" xr3:uid="{4974749D-575F-4937-BCDB-A5BF814F4AC6}" uniqueName="16" name="Column1.16" queryTableFieldId="16" dataDxfId="53"/>
-    <tableColumn id="17" xr3:uid="{6E5F205B-628F-4E9E-8798-A6D2ABEDE903}" uniqueName="17" name="Column1.17" queryTableFieldId="17" dataDxfId="52"/>
-    <tableColumn id="18" xr3:uid="{33BF4F05-522D-4A98-A15A-C2F028B9CB80}" uniqueName="18" name="Column1.18" queryTableFieldId="18" dataDxfId="51"/>
-    <tableColumn id="19" xr3:uid="{02691FAC-5D3C-46A3-98DB-CD8E9C5AB728}" uniqueName="19" name="Column1.19" queryTableFieldId="19" dataDxfId="50"/>
-    <tableColumn id="20" xr3:uid="{C6CA6DEF-09A3-4585-98CC-29839DAF6065}" uniqueName="20" name="Column1.20" queryTableFieldId="20" dataDxfId="49"/>
-    <tableColumn id="21" xr3:uid="{01B142FC-2EB4-420F-86F3-3B9283FDB718}" uniqueName="21" name="Column1.21" queryTableFieldId="21" dataDxfId="48"/>
-    <tableColumn id="22" xr3:uid="{B7CF140E-856F-4589-8798-75C605274AEC}" uniqueName="22" name="Column1.22" queryTableFieldId="22" dataDxfId="47"/>
-    <tableColumn id="23" xr3:uid="{951BD0E2-DDFD-4290-AA0B-58C28F861ABA}" uniqueName="23" name="Column1.23" queryTableFieldId="23" dataDxfId="46"/>
-    <tableColumn id="24" xr3:uid="{6C88DDE6-BCAF-483D-8F88-A95D05524297}" uniqueName="24" name="Column1.24" queryTableFieldId="24" dataDxfId="45"/>
-    <tableColumn id="25" xr3:uid="{C1ABB74C-8AA7-4FCA-918A-7870A2E05231}" uniqueName="25" name="Column1.25" queryTableFieldId="25" dataDxfId="44"/>
-    <tableColumn id="26" xr3:uid="{A6FB7780-F4E3-4457-9A1D-5FC379DD2C69}" uniqueName="26" name="Column1.26" queryTableFieldId="26" dataDxfId="43"/>
-    <tableColumn id="27" xr3:uid="{509A6CB3-AA4E-408D-97A0-EB0E19E864C9}" uniqueName="27" name="Column1.27" queryTableFieldId="27" dataDxfId="42"/>
-    <tableColumn id="28" xr3:uid="{C7C161BA-BE21-4AAC-8649-870342CB946E}" uniqueName="28" name="Column1.28" queryTableFieldId="28" dataDxfId="41"/>
-    <tableColumn id="29" xr3:uid="{AF6A9937-CDFB-4706-B055-F4C798B14BB1}" uniqueName="29" name="Column1.29" queryTableFieldId="29" dataDxfId="40"/>
-    <tableColumn id="30" xr3:uid="{96F53ACE-2A8C-471F-82BC-7359316BC210}" uniqueName="30" name="Column1.30" queryTableFieldId="30" dataDxfId="39"/>
-    <tableColumn id="31" xr3:uid="{A7B45218-0F7F-412F-9D8E-37CAF6305EA7}" uniqueName="31" name="Column1.31" queryTableFieldId="31" dataDxfId="38"/>
-    <tableColumn id="32" xr3:uid="{8F551DE8-5C44-420F-B251-B349A9EC051D}" uniqueName="32" name="Column1.32" queryTableFieldId="32" dataDxfId="37"/>
-    <tableColumn id="33" xr3:uid="{02E1FD0A-8E68-4B39-91B3-58C86518AE57}" uniqueName="33" name="Column1.33" queryTableFieldId="33" dataDxfId="36"/>
-    <tableColumn id="34" xr3:uid="{80BB6666-7C1B-4288-B066-4B33AB2126E1}" uniqueName="34" name="Column1.34" queryTableFieldId="34" dataDxfId="35"/>
-    <tableColumn id="35" xr3:uid="{343F525E-D77A-439B-8080-B298C5A9A8A9}" uniqueName="35" name="Column1.35" queryTableFieldId="35" dataDxfId="34"/>
-    <tableColumn id="36" xr3:uid="{2C64F378-4F69-45B7-A855-7B0F18458638}" uniqueName="36" name="Column1.36" queryTableFieldId="36" dataDxfId="33"/>
-    <tableColumn id="37" xr3:uid="{3B9F7BCA-E16F-41FA-9127-8D9449348ACD}" uniqueName="37" name="Column1.37" queryTableFieldId="37" dataDxfId="32"/>
-    <tableColumn id="38" xr3:uid="{7D220A03-AB25-4024-BFB5-D259C022D689}" uniqueName="38" name="Column1.38" queryTableFieldId="38" dataDxfId="31"/>
-    <tableColumn id="39" xr3:uid="{39D1F24C-FED1-42E9-B265-864CFB7E9423}" uniqueName="39" name="Column1.39" queryTableFieldId="39" dataDxfId="30"/>
-    <tableColumn id="40" xr3:uid="{E9A375CA-F4FB-4763-A6B7-E9E3809C4043}" uniqueName="40" name="Column1.40" queryTableFieldId="40" dataDxfId="29"/>
-    <tableColumn id="41" xr3:uid="{9AD88CE7-4122-4110-9862-C565102D85A0}" uniqueName="41" name="Column1.41" queryTableFieldId="41" dataDxfId="28"/>
-    <tableColumn id="42" xr3:uid="{4FAE40BB-3BE4-4533-98E6-8F7B02206EC9}" uniqueName="42" name="Column1.42" queryTableFieldId="42" dataDxfId="27"/>
-    <tableColumn id="43" xr3:uid="{01691B36-C05A-47D3-9F63-3192B61D88AF}" uniqueName="43" name="Column1.43" queryTableFieldId="43" dataDxfId="26"/>
-    <tableColumn id="44" xr3:uid="{42479B0A-E0A8-426E-849A-7E051548D1D3}" uniqueName="44" name="Column1.44" queryTableFieldId="44" dataDxfId="25"/>
-    <tableColumn id="45" xr3:uid="{1803487B-30B4-4DB7-8C32-FED9CF86FBE7}" uniqueName="45" name="Column1.45" queryTableFieldId="45" dataDxfId="24"/>
-    <tableColumn id="46" xr3:uid="{68AA4A33-75D3-417B-BD7A-613E00647A54}" uniqueName="46" name="Column1.46" queryTableFieldId="46" dataDxfId="23"/>
-    <tableColumn id="47" xr3:uid="{D72DEFDB-64CF-4AB1-B8D9-AAE87C1FCBB8}" uniqueName="47" name="Column1.47" queryTableFieldId="47" dataDxfId="22"/>
-    <tableColumn id="48" xr3:uid="{4920831C-6FCF-4CCE-8730-4F19D7836288}" uniqueName="48" name="Column1.48" queryTableFieldId="48" dataDxfId="21"/>
-    <tableColumn id="49" xr3:uid="{FEFDF036-3127-4540-B5FE-9646BE021522}" uniqueName="49" name="Column1.49" queryTableFieldId="49" dataDxfId="20"/>
-    <tableColumn id="50" xr3:uid="{ED218BF8-F986-48DC-B2E3-30D805227D0B}" uniqueName="50" name="Column1.50" queryTableFieldId="50" dataDxfId="19"/>
-    <tableColumn id="51" xr3:uid="{F2F34919-1283-42FA-98C1-AAF0F87FB4FB}" uniqueName="51" name="Column1.51" queryTableFieldId="51" dataDxfId="18"/>
-    <tableColumn id="52" xr3:uid="{7C290BBB-A571-499D-9333-47CB4D02007D}" uniqueName="52" name="Column1.52" queryTableFieldId="52" dataDxfId="17"/>
-    <tableColumn id="53" xr3:uid="{4248EF63-58F7-4AAB-9FD0-4F10033C1E07}" uniqueName="53" name="Column1.53" queryTableFieldId="53" dataDxfId="16"/>
-    <tableColumn id="54" xr3:uid="{8A141472-EC69-450D-9307-98952DDA3E3C}" uniqueName="54" name="Column1.54" queryTableFieldId="54" dataDxfId="15"/>
-    <tableColumn id="55" xr3:uid="{27418C71-D4A7-425C-BE5D-14BA8619C378}" uniqueName="55" name="Column1.55" queryTableFieldId="55" dataDxfId="14"/>
-    <tableColumn id="56" xr3:uid="{A3BB11A4-A297-4A64-909A-D5C7F90D23F2}" uniqueName="56" name="Column1.56" queryTableFieldId="56" dataDxfId="13"/>
-    <tableColumn id="57" xr3:uid="{0761E0B7-55B6-448B-8B63-D8816E0E5E50}" uniqueName="57" name="Column1.57" queryTableFieldId="57" dataDxfId="12"/>
-    <tableColumn id="58" xr3:uid="{2112CDC5-0036-43C0-A4A7-991A2466B65A}" uniqueName="58" name="Column1.58" queryTableFieldId="58" dataDxfId="11"/>
-    <tableColumn id="59" xr3:uid="{FA399E72-80A1-4836-B05E-8E6BFE3A459F}" uniqueName="59" name="Column1.59" queryTableFieldId="59" dataDxfId="10"/>
-    <tableColumn id="60" xr3:uid="{258EFBB5-3989-4746-A02F-8E1ED88AA915}" uniqueName="60" name="Column1.60" queryTableFieldId="60" dataDxfId="9"/>
-    <tableColumn id="61" xr3:uid="{00A8BF95-E157-4740-AA82-19E0565B6493}" uniqueName="61" name="Column1.61" queryTableFieldId="61" dataDxfId="8"/>
-    <tableColumn id="62" xr3:uid="{2F005A1B-FF17-419C-BC06-230389DE0AF3}" uniqueName="62" name="Column1.62" queryTableFieldId="62" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{98D7E3A4-39DE-47DA-B944-49F0A0557E5E}" uniqueName="1" name="Column1.1" queryTableFieldId="1" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{509FB6ED-99F2-4BA7-88F1-D89840A7811D}" uniqueName="2" name="Column1.2" queryTableFieldId="2" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{419A591C-63BF-414F-BA41-385855C462C5}" uniqueName="3" name="Column1.3" queryTableFieldId="3" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{314CDC71-6274-4F19-B9F7-6415F8BA4687}" uniqueName="4" name="Column1.4" queryTableFieldId="4" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{6833C0D6-8864-420C-BE0E-1074B5CC7001}" uniqueName="5" name="Column1.5" queryTableFieldId="5" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{500A35EC-ECFA-4C32-A548-3FCC313C4F84}" uniqueName="6" name="Column1.6" queryTableFieldId="6" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{B3D8B8ED-1C0E-4F03-9ECB-9AC46B3CD351}" uniqueName="7" name="Column1.7" queryTableFieldId="7" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{CBCC21E0-9F71-40A0-AEAA-592F841E8838}" uniqueName="8" name="Column1.8" queryTableFieldId="8" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{54B3DF67-DE7B-4698-A77F-9B809ABF105F}" uniqueName="9" name="Column1.9" queryTableFieldId="9" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{1F4B4B60-7C8A-4787-93DA-BEA5BCBC30E0}" uniqueName="10" name="Column1.10" queryTableFieldId="10" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{B8AF0B34-E3D2-448B-99BE-4BA87ECF720C}" uniqueName="11" name="Column1.11" queryTableFieldId="11" dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{BAABB28F-07F3-43A6-95AF-5AE4E22ADFC3}" uniqueName="12" name="Column1.12" queryTableFieldId="12" dataDxfId="50"/>
+    <tableColumn id="13" xr3:uid="{6519F06B-2422-425E-8296-23A84F1F2FFE}" uniqueName="13" name="Column1.13" queryTableFieldId="13" dataDxfId="49"/>
+    <tableColumn id="14" xr3:uid="{2CB1F290-4BBD-4E61-B61D-46BDB8CE41FA}" uniqueName="14" name="Column1.14" queryTableFieldId="14" dataDxfId="48"/>
+    <tableColumn id="15" xr3:uid="{74E4D9B8-6A6C-45A1-BECA-E84B35CD2549}" uniqueName="15" name="Column1.15" queryTableFieldId="15" dataDxfId="47"/>
+    <tableColumn id="16" xr3:uid="{4974749D-575F-4937-BCDB-A5BF814F4AC6}" uniqueName="16" name="Column1.16" queryTableFieldId="16" dataDxfId="46"/>
+    <tableColumn id="17" xr3:uid="{6E5F205B-628F-4E9E-8798-A6D2ABEDE903}" uniqueName="17" name="Column1.17" queryTableFieldId="17" dataDxfId="45"/>
+    <tableColumn id="18" xr3:uid="{33BF4F05-522D-4A98-A15A-C2F028B9CB80}" uniqueName="18" name="Column1.18" queryTableFieldId="18" dataDxfId="44"/>
+    <tableColumn id="19" xr3:uid="{02691FAC-5D3C-46A3-98DB-CD8E9C5AB728}" uniqueName="19" name="Column1.19" queryTableFieldId="19" dataDxfId="43"/>
+    <tableColumn id="20" xr3:uid="{C6CA6DEF-09A3-4585-98CC-29839DAF6065}" uniqueName="20" name="Column1.20" queryTableFieldId="20" dataDxfId="42"/>
+    <tableColumn id="21" xr3:uid="{01B142FC-2EB4-420F-86F3-3B9283FDB718}" uniqueName="21" name="Column1.21" queryTableFieldId="21" dataDxfId="41"/>
+    <tableColumn id="22" xr3:uid="{B7CF140E-856F-4589-8798-75C605274AEC}" uniqueName="22" name="Column1.22" queryTableFieldId="22" dataDxfId="40"/>
+    <tableColumn id="23" xr3:uid="{951BD0E2-DDFD-4290-AA0B-58C28F861ABA}" uniqueName="23" name="Column1.23" queryTableFieldId="23" dataDxfId="39"/>
+    <tableColumn id="24" xr3:uid="{6C88DDE6-BCAF-483D-8F88-A95D05524297}" uniqueName="24" name="Column1.24" queryTableFieldId="24" dataDxfId="38"/>
+    <tableColumn id="25" xr3:uid="{C1ABB74C-8AA7-4FCA-918A-7870A2E05231}" uniqueName="25" name="Column1.25" queryTableFieldId="25" dataDxfId="37"/>
+    <tableColumn id="26" xr3:uid="{A6FB7780-F4E3-4457-9A1D-5FC379DD2C69}" uniqueName="26" name="Column1.26" queryTableFieldId="26" dataDxfId="36"/>
+    <tableColumn id="27" xr3:uid="{509A6CB3-AA4E-408D-97A0-EB0E19E864C9}" uniqueName="27" name="Column1.27" queryTableFieldId="27" dataDxfId="35"/>
+    <tableColumn id="28" xr3:uid="{C7C161BA-BE21-4AAC-8649-870342CB946E}" uniqueName="28" name="Column1.28" queryTableFieldId="28" dataDxfId="34"/>
+    <tableColumn id="29" xr3:uid="{AF6A9937-CDFB-4706-B055-F4C798B14BB1}" uniqueName="29" name="Column1.29" queryTableFieldId="29" dataDxfId="33"/>
+    <tableColumn id="30" xr3:uid="{96F53ACE-2A8C-471F-82BC-7359316BC210}" uniqueName="30" name="Column1.30" queryTableFieldId="30" dataDxfId="32"/>
+    <tableColumn id="31" xr3:uid="{A7B45218-0F7F-412F-9D8E-37CAF6305EA7}" uniqueName="31" name="Column1.31" queryTableFieldId="31" dataDxfId="31"/>
+    <tableColumn id="32" xr3:uid="{8F551DE8-5C44-420F-B251-B349A9EC051D}" uniqueName="32" name="Column1.32" queryTableFieldId="32" dataDxfId="30"/>
+    <tableColumn id="33" xr3:uid="{02E1FD0A-8E68-4B39-91B3-58C86518AE57}" uniqueName="33" name="Column1.33" queryTableFieldId="33" dataDxfId="29"/>
+    <tableColumn id="34" xr3:uid="{80BB6666-7C1B-4288-B066-4B33AB2126E1}" uniqueName="34" name="Column1.34" queryTableFieldId="34" dataDxfId="28"/>
+    <tableColumn id="35" xr3:uid="{343F525E-D77A-439B-8080-B298C5A9A8A9}" uniqueName="35" name="Column1.35" queryTableFieldId="35" dataDxfId="27"/>
+    <tableColumn id="36" xr3:uid="{2C64F378-4F69-45B7-A855-7B0F18458638}" uniqueName="36" name="Column1.36" queryTableFieldId="36" dataDxfId="26"/>
+    <tableColumn id="37" xr3:uid="{3B9F7BCA-E16F-41FA-9127-8D9449348ACD}" uniqueName="37" name="Column1.37" queryTableFieldId="37" dataDxfId="25"/>
+    <tableColumn id="38" xr3:uid="{7D220A03-AB25-4024-BFB5-D259C022D689}" uniqueName="38" name="Column1.38" queryTableFieldId="38" dataDxfId="24"/>
+    <tableColumn id="39" xr3:uid="{39D1F24C-FED1-42E9-B265-864CFB7E9423}" uniqueName="39" name="Column1.39" queryTableFieldId="39" dataDxfId="23"/>
+    <tableColumn id="40" xr3:uid="{E9A375CA-F4FB-4763-A6B7-E9E3809C4043}" uniqueName="40" name="Column1.40" queryTableFieldId="40" dataDxfId="22"/>
+    <tableColumn id="41" xr3:uid="{9AD88CE7-4122-4110-9862-C565102D85A0}" uniqueName="41" name="Column1.41" queryTableFieldId="41" dataDxfId="21"/>
+    <tableColumn id="42" xr3:uid="{4FAE40BB-3BE4-4533-98E6-8F7B02206EC9}" uniqueName="42" name="Column1.42" queryTableFieldId="42" dataDxfId="20"/>
+    <tableColumn id="43" xr3:uid="{01691B36-C05A-47D3-9F63-3192B61D88AF}" uniqueName="43" name="Column1.43" queryTableFieldId="43" dataDxfId="19"/>
+    <tableColumn id="44" xr3:uid="{42479B0A-E0A8-426E-849A-7E051548D1D3}" uniqueName="44" name="Column1.44" queryTableFieldId="44" dataDxfId="18"/>
+    <tableColumn id="45" xr3:uid="{1803487B-30B4-4DB7-8C32-FED9CF86FBE7}" uniqueName="45" name="Column1.45" queryTableFieldId="45" dataDxfId="17"/>
+    <tableColumn id="46" xr3:uid="{68AA4A33-75D3-417B-BD7A-613E00647A54}" uniqueName="46" name="Column1.46" queryTableFieldId="46" dataDxfId="16"/>
+    <tableColumn id="47" xr3:uid="{D72DEFDB-64CF-4AB1-B8D9-AAE87C1FCBB8}" uniqueName="47" name="Column1.47" queryTableFieldId="47" dataDxfId="15"/>
+    <tableColumn id="48" xr3:uid="{4920831C-6FCF-4CCE-8730-4F19D7836288}" uniqueName="48" name="Column1.48" queryTableFieldId="48" dataDxfId="14"/>
+    <tableColumn id="49" xr3:uid="{FEFDF036-3127-4540-B5FE-9646BE021522}" uniqueName="49" name="Column1.49" queryTableFieldId="49" dataDxfId="13"/>
+    <tableColumn id="50" xr3:uid="{ED218BF8-F986-48DC-B2E3-30D805227D0B}" uniqueName="50" name="Column1.50" queryTableFieldId="50" dataDxfId="12"/>
+    <tableColumn id="51" xr3:uid="{F2F34919-1283-42FA-98C1-AAF0F87FB4FB}" uniqueName="51" name="Column1.51" queryTableFieldId="51" dataDxfId="11"/>
+    <tableColumn id="52" xr3:uid="{7C290BBB-A571-499D-9333-47CB4D02007D}" uniqueName="52" name="Column1.52" queryTableFieldId="52" dataDxfId="10"/>
+    <tableColumn id="53" xr3:uid="{4248EF63-58F7-4AAB-9FD0-4F10033C1E07}" uniqueName="53" name="Column1.53" queryTableFieldId="53" dataDxfId="9"/>
+    <tableColumn id="54" xr3:uid="{8A141472-EC69-450D-9307-98952DDA3E3C}" uniqueName="54" name="Column1.54" queryTableFieldId="54" dataDxfId="8"/>
+    <tableColumn id="55" xr3:uid="{27418C71-D4A7-425C-BE5D-14BA8619C378}" uniqueName="55" name="Column1.55" queryTableFieldId="55" dataDxfId="7"/>
+    <tableColumn id="56" xr3:uid="{A3BB11A4-A297-4A64-909A-D5C7F90D23F2}" uniqueName="56" name="Column1.56" queryTableFieldId="56" dataDxfId="6"/>
+    <tableColumn id="57" xr3:uid="{0761E0B7-55B6-448B-8B63-D8816E0E5E50}" uniqueName="57" name="Column1.57" queryTableFieldId="57" dataDxfId="5"/>
+    <tableColumn id="58" xr3:uid="{2112CDC5-0036-43C0-A4A7-991A2466B65A}" uniqueName="58" name="Column1.58" queryTableFieldId="58" dataDxfId="4"/>
+    <tableColumn id="59" xr3:uid="{FA399E72-80A1-4836-B05E-8E6BFE3A459F}" uniqueName="59" name="Column1.59" queryTableFieldId="59" dataDxfId="3"/>
+    <tableColumn id="60" xr3:uid="{258EFBB5-3989-4746-A02F-8E1ED88AA915}" uniqueName="60" name="Column1.60" queryTableFieldId="60" dataDxfId="2"/>
+    <tableColumn id="61" xr3:uid="{00A8BF95-E157-4740-AA82-19E0565B6493}" uniqueName="61" name="Column1.61" queryTableFieldId="61" dataDxfId="1"/>
+    <tableColumn id="62" xr3:uid="{2F005A1B-FF17-419C-BC06-230389DE0AF3}" uniqueName="62" name="Column1.62" queryTableFieldId="62" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2394,8 +2393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554198ED-48BB-4219-B73C-9BDA64B3C366}">
   <dimension ref="A1:BJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BI62" sqref="B3:BI62"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:BI62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6510,7 +6509,7 @@
         <v>2</v>
       </c>
       <c r="BB22" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC22" s="1" t="s">
         <v>5</v>
@@ -11398,7 +11397,7 @@
         <v>2</v>
       </c>
       <c r="BB48" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC48" s="1" t="s">
         <v>0</v>
@@ -12520,10 +12519,10 @@
         <v>2</v>
       </c>
       <c r="AZ54" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BA54" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BB54" s="1" t="s">
         <v>1</v>
@@ -14241,27 +14240,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="T">
+    <cfRule type="containsText" dxfId="190" priority="1" operator="containsText" text="T">
       <formula>NOT(ISERROR(SEARCH("T",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="189" priority="3" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH("B",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="G">
+    <cfRule type="containsText" dxfId="188" priority="4" operator="containsText" text="G">
       <formula>NOT(ISERROR(SEARCH("G",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="z">
+    <cfRule type="containsText" dxfId="187" priority="5" operator="containsText" text="z">
       <formula>NOT(ISERROR(SEARCH("z",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="186" priority="6" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="185" priority="7" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P26">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="T">
+    <cfRule type="containsText" dxfId="184" priority="2" operator="containsText" text="T">
       <formula>NOT(ISERROR(SEARCH("T",P26)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25394,7 +25393,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE09672-E204-41DF-8915-BF62C46A03E5}">
-  <dimension ref="A1:BJ3"/>
+  <dimension ref="A1:BJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -25595,256 +25594,192 @@
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="6" t="s">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="6" t="s">
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AC2" t="s">
         <v>3</v>
       </c>
-      <c r="AD2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AY2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="AD2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>3</v>
       </c>
-      <c r="BA2" s="6" t="s">
+      <c r="BA2" t="s">
         <v>3</v>
       </c>
-      <c r="BB2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="BC2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="BD2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="BE2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="BF2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BG2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BH2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="BI2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="BJ2" s="6" t="s">
+      <c r="BB2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6"/>
-      <c r="AL3" s="6"/>
-      <c r="AM3" s="6"/>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="6"/>
-      <c r="AP3" s="6"/>
-      <c r="AQ3" s="6"/>
-      <c r="AR3" s="6"/>
-      <c r="AS3" s="6"/>
-      <c r="AT3" s="6"/>
-      <c r="AU3" s="6"/>
-      <c r="AV3" s="6"/>
-      <c r="AW3" s="6"/>
-      <c r="AX3" s="6"/>
-      <c r="AY3" s="6"/>
-      <c r="AZ3" s="6"/>
-      <c r="BA3" s="6"/>
-      <c r="BB3" s="6"/>
-      <c r="BC3" s="6"/>
-      <c r="BD3" s="6"/>
-      <c r="BE3" s="6"/>
-      <c r="BF3" s="6"/>
-      <c r="BG3" s="6"/>
-      <c r="BH3" s="6"/>
-      <c r="BI3" s="6"/>
-      <c r="BJ3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>